<commit_message>
Feat: Agrega clase de validacion de datos
</commit_message>
<xml_diff>
--- a/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
+++ b/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\codev\dev\projects\learning\data-analyst\excel-intermedio-tableros-formulas\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBD9239-3B02-46DA-BFE7-56B63073CDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA808DB-996E-47C4-9626-B5DED0B9DF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" firstSheet="3" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ventas" sheetId="3" r:id="rId1"/>
@@ -213,7 +213,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -293,9 +293,9 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C0ADA3-4C22-4CF9-8AD3-3A127D5F6CB1}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4176,741 +4176,93 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="3">
-        <v>44568</v>
-      </c>
-      <c r="B153" s="4">
-        <v>5649.31</v>
-      </c>
-      <c r="C153" s="4">
-        <v>4933.16</v>
-      </c>
-      <c r="D153" s="4">
-        <v>716.15</v>
-      </c>
-      <c r="E153" s="4">
-        <v>0</v>
-      </c>
-      <c r="F153" s="4">
-        <v>2779.85</v>
-      </c>
-      <c r="G153">
-        <v>59</v>
-      </c>
+      <c r="A153"/>
+      <c r="B153"/>
+      <c r="C153"/>
+      <c r="D153"/>
+      <c r="E153"/>
+      <c r="F153"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="3">
-        <v>44575</v>
-      </c>
-      <c r="B154" s="4">
-        <v>3503.12</v>
-      </c>
-      <c r="C154" s="4">
-        <v>2831.55</v>
-      </c>
-      <c r="D154" s="4">
-        <v>671.57</v>
-      </c>
-      <c r="E154" s="4">
-        <v>0</v>
-      </c>
-      <c r="F154" s="4">
-        <v>1996.33</v>
-      </c>
-      <c r="G154">
-        <v>33</v>
-      </c>
+      <c r="A154"/>
+      <c r="B154"/>
+      <c r="C154"/>
+      <c r="D154"/>
+      <c r="E154"/>
+      <c r="F154"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="3">
-        <v>44576</v>
-      </c>
-      <c r="B155" s="4">
-        <v>6727.53</v>
-      </c>
-      <c r="C155" s="4">
-        <v>5752.18</v>
-      </c>
-      <c r="D155" s="4">
-        <v>975.35</v>
-      </c>
-      <c r="E155" s="4">
-        <v>0</v>
-      </c>
-      <c r="F155" s="4">
-        <v>3750.84</v>
-      </c>
-      <c r="G155">
-        <v>48</v>
-      </c>
+      <c r="A155"/>
+      <c r="B155"/>
+      <c r="C155"/>
+      <c r="D155"/>
+      <c r="E155"/>
+      <c r="F155"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="3">
-        <v>44577</v>
-      </c>
-      <c r="B156" s="4">
-        <v>3620.16</v>
-      </c>
-      <c r="C156" s="4">
-        <v>3216.57</v>
-      </c>
-      <c r="D156" s="4">
-        <v>403.59</v>
-      </c>
-      <c r="E156" s="4">
-        <v>0</v>
-      </c>
-      <c r="F156" s="4">
-        <v>2127.77</v>
-      </c>
-      <c r="G156">
-        <v>28</v>
-      </c>
+      <c r="A156"/>
+      <c r="B156"/>
+      <c r="C156"/>
+      <c r="D156"/>
+      <c r="E156"/>
+      <c r="F156"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="3">
-        <v>44616</v>
-      </c>
-      <c r="B157" s="4">
-        <v>4088.09</v>
-      </c>
-      <c r="C157" s="4">
-        <v>3492.17</v>
-      </c>
-      <c r="D157" s="4">
-        <v>595.91999999999996</v>
-      </c>
-      <c r="E157" s="4">
-        <v>0</v>
-      </c>
-      <c r="F157" s="4">
-        <v>2317.0700000000002</v>
-      </c>
-      <c r="G157">
-        <v>40</v>
-      </c>
+      <c r="A157"/>
+      <c r="B157"/>
+      <c r="C157"/>
+      <c r="D157"/>
+      <c r="E157"/>
+      <c r="F157"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="3">
-        <v>44617</v>
-      </c>
-      <c r="B158" s="4">
-        <v>2918.34</v>
-      </c>
-      <c r="C158" s="4">
-        <v>2489.85</v>
-      </c>
-      <c r="D158" s="4">
-        <v>428.49</v>
-      </c>
-      <c r="E158" s="4">
-        <v>0</v>
-      </c>
-      <c r="F158" s="4">
-        <v>1668.94</v>
-      </c>
-      <c r="G158">
-        <v>34</v>
-      </c>
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="C158"/>
+      <c r="D158"/>
+      <c r="E158"/>
+      <c r="F158"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="3">
-        <v>44618</v>
-      </c>
-      <c r="B159" s="4">
-        <v>7506.01</v>
-      </c>
-      <c r="C159" s="4">
-        <v>4240.6499999999996</v>
-      </c>
-      <c r="D159" s="4">
-        <v>3265.36</v>
-      </c>
-      <c r="E159" s="4">
-        <v>0</v>
-      </c>
-      <c r="F159" s="4">
-        <v>4222.74</v>
-      </c>
-      <c r="G159">
-        <v>49</v>
-      </c>
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="C159"/>
+      <c r="D159"/>
+      <c r="E159"/>
+      <c r="F159"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="3">
-        <v>44628</v>
-      </c>
-      <c r="B160" s="4">
-        <v>5725.4</v>
-      </c>
-      <c r="C160" s="4">
-        <v>4397.01</v>
-      </c>
-      <c r="D160" s="4">
-        <v>1328.39</v>
-      </c>
-      <c r="E160" s="4">
-        <v>0</v>
-      </c>
-      <c r="F160" s="4">
-        <v>3161.2</v>
-      </c>
-      <c r="G160">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="3">
-        <v>44658</v>
-      </c>
-      <c r="B161" s="4">
-        <v>4385.3500000000004</v>
-      </c>
-      <c r="C161" s="4">
-        <v>4385.3500000000004</v>
-      </c>
-      <c r="D161" s="4">
-        <v>0</v>
-      </c>
-      <c r="E161" s="4">
-        <v>0</v>
-      </c>
-      <c r="F161" s="4">
-        <v>2619.86</v>
-      </c>
-      <c r="G161">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" s="3">
-        <v>44659</v>
-      </c>
-      <c r="B162" s="4">
-        <v>4999.97</v>
-      </c>
-      <c r="C162" s="4">
-        <v>3970.51</v>
-      </c>
-      <c r="D162" s="4">
-        <v>1029.46</v>
-      </c>
-      <c r="E162" s="4">
-        <v>0</v>
-      </c>
-      <c r="F162" s="4">
-        <v>2937.99</v>
-      </c>
-      <c r="G162">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="3">
-        <v>44660</v>
-      </c>
-      <c r="B163" s="4">
-        <v>4886.8999999999996</v>
-      </c>
-      <c r="C163" s="4">
-        <v>3893.99</v>
-      </c>
-      <c r="D163" s="4">
-        <v>992.91</v>
-      </c>
-      <c r="E163" s="4">
-        <v>0</v>
-      </c>
-      <c r="F163" s="4">
-        <v>2862.35</v>
-      </c>
-      <c r="G163">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" s="3">
-        <v>44572</v>
-      </c>
-      <c r="B164" s="4">
-        <v>4226.25</v>
-      </c>
-      <c r="C164" s="4">
-        <v>3692.89</v>
-      </c>
-      <c r="D164" s="4">
-        <v>533.36</v>
-      </c>
-      <c r="E164" s="4">
-        <v>0</v>
-      </c>
-      <c r="F164" s="4">
-        <v>2411.77</v>
-      </c>
-      <c r="G164">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="3">
-        <v>44573</v>
-      </c>
-      <c r="B165" s="4">
-        <v>4172.46</v>
-      </c>
-      <c r="C165" s="4">
-        <v>4172.46</v>
-      </c>
-      <c r="D165" s="4">
-        <v>0</v>
-      </c>
-      <c r="E165" s="4">
-        <v>0</v>
-      </c>
-      <c r="F165" s="4">
-        <v>2291.9499999999998</v>
-      </c>
-      <c r="G165">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="3">
-        <v>44580</v>
-      </c>
-      <c r="B166" s="4">
-        <v>3966.48</v>
-      </c>
-      <c r="C166" s="4">
-        <v>3605.21</v>
-      </c>
-      <c r="D166" s="4">
-        <v>361.27</v>
-      </c>
-      <c r="E166" s="4">
-        <v>0</v>
-      </c>
-      <c r="F166" s="4">
-        <v>2216.8200000000002</v>
-      </c>
-      <c r="G166">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="3">
-        <v>44592</v>
-      </c>
-      <c r="B167" s="4">
-        <v>4221.26</v>
-      </c>
-      <c r="C167" s="4">
-        <v>4169.25</v>
-      </c>
-      <c r="D167" s="4">
-        <v>52.01</v>
-      </c>
-      <c r="E167" s="4">
-        <v>0</v>
-      </c>
-      <c r="F167" s="4">
-        <v>2391.35</v>
-      </c>
-      <c r="G167">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" s="3">
-        <v>44598</v>
-      </c>
-      <c r="B168" s="4">
-        <v>2630.46</v>
-      </c>
-      <c r="C168" s="4">
-        <v>1803.43</v>
-      </c>
-      <c r="D168" s="4">
-        <v>827.03</v>
-      </c>
-      <c r="E168" s="4">
-        <v>0</v>
-      </c>
-      <c r="F168" s="4">
-        <v>1669.58</v>
-      </c>
-      <c r="G168">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="3">
-        <v>44605</v>
-      </c>
-      <c r="B169" s="4">
-        <v>2562.7199999999998</v>
-      </c>
-      <c r="C169" s="4">
-        <v>2031.79</v>
-      </c>
-      <c r="D169" s="4">
-        <v>530.92999999999995</v>
-      </c>
-      <c r="E169" s="4">
-        <v>0</v>
-      </c>
-      <c r="F169" s="4">
-        <v>1417.57</v>
-      </c>
-      <c r="G169">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" s="3">
-        <v>44607</v>
-      </c>
-      <c r="B170" s="4">
-        <v>6054.22</v>
-      </c>
-      <c r="C170" s="4">
-        <v>5314.25</v>
-      </c>
-      <c r="D170" s="4">
-        <v>739.97</v>
-      </c>
-      <c r="E170" s="4">
-        <v>0</v>
-      </c>
-      <c r="F170" s="4">
-        <v>3472.59</v>
-      </c>
-      <c r="G170">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="3">
-        <v>44618</v>
-      </c>
-      <c r="B171" s="4">
-        <v>7506.01</v>
-      </c>
-      <c r="C171" s="4">
-        <v>4240.6499999999996</v>
-      </c>
-      <c r="D171" s="4">
-        <v>3265.36</v>
-      </c>
-      <c r="E171" s="4">
-        <v>0</v>
-      </c>
-      <c r="F171" s="4">
-        <v>4222.74</v>
-      </c>
-      <c r="G171">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="3">
-        <v>44622</v>
-      </c>
-      <c r="B172" s="4">
-        <v>2966.54</v>
-      </c>
-      <c r="C172" s="4">
-        <v>2898.01</v>
-      </c>
-      <c r="D172" s="4">
-        <v>68.53</v>
-      </c>
-      <c r="E172" s="4">
-        <v>0</v>
-      </c>
-      <c r="F172" s="4">
-        <v>0</v>
-      </c>
-      <c r="G172">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="3">
-        <v>44630</v>
-      </c>
-      <c r="B173" s="4">
-        <v>3606.48</v>
-      </c>
-      <c r="C173" s="4">
-        <v>3297.16</v>
-      </c>
-      <c r="D173" s="4">
-        <v>309.32</v>
-      </c>
-      <c r="E173" s="4">
-        <v>0</v>
-      </c>
-      <c r="F173" s="4">
-        <v>2165.2199999999998</v>
-      </c>
-      <c r="G173">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="3">
-        <v>44639</v>
-      </c>
-      <c r="B174" s="4">
-        <v>3686.54</v>
-      </c>
-      <c r="C174" s="4">
-        <v>3434.56</v>
-      </c>
-      <c r="D174" s="4">
-        <v>251.98</v>
-      </c>
-      <c r="E174" s="4">
-        <v>0</v>
-      </c>
-      <c r="F174" s="4">
-        <v>2280.5</v>
-      </c>
-      <c r="G174">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A175" s="3">
-        <v>44650</v>
-      </c>
-      <c r="B175" s="4">
-        <v>2922.44</v>
-      </c>
-      <c r="C175" s="4">
-        <v>2621.94</v>
-      </c>
-      <c r="D175" s="4">
-        <v>300.5</v>
-      </c>
-      <c r="E175" s="4">
-        <v>0</v>
-      </c>
-      <c r="F175" s="4">
-        <v>1680.93</v>
-      </c>
-      <c r="G175">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="3">
-        <v>44665</v>
-      </c>
-      <c r="B176" s="4">
-        <v>2113.21</v>
-      </c>
-      <c r="C176" s="4">
-        <v>1467.32</v>
-      </c>
-      <c r="D176" s="4">
-        <v>645.89</v>
-      </c>
-      <c r="E176" s="4">
-        <v>0</v>
-      </c>
-      <c r="F176" s="4">
-        <v>1275.03</v>
-      </c>
-      <c r="G176">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="3">
-        <v>44688</v>
-      </c>
-      <c r="B177" s="4">
-        <v>3771.87</v>
-      </c>
-      <c r="C177" s="4">
-        <v>3606.46</v>
-      </c>
-      <c r="D177" s="4">
-        <v>165.41</v>
-      </c>
-      <c r="E177" s="4">
-        <v>0</v>
-      </c>
-      <c r="F177" s="4">
-        <v>2210.9</v>
-      </c>
-      <c r="G177">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" s="3">
-        <v>44692</v>
-      </c>
-      <c r="B178" s="4">
-        <v>2697</v>
-      </c>
-      <c r="C178" s="4">
-        <v>2265.39</v>
-      </c>
-      <c r="D178" s="4">
-        <v>431.61</v>
-      </c>
-      <c r="E178" s="4">
-        <v>0</v>
-      </c>
-      <c r="F178" s="4">
-        <v>1614.29</v>
-      </c>
-      <c r="G178">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="3">
-        <v>44693</v>
-      </c>
-      <c r="B179" s="4">
-        <v>5016.97</v>
-      </c>
-      <c r="C179" s="4">
-        <v>3192.75</v>
-      </c>
-      <c r="D179" s="4">
-        <v>1824.22</v>
-      </c>
-      <c r="E179" s="4">
-        <v>0</v>
-      </c>
-      <c r="F179" s="4">
-        <v>2935.17</v>
-      </c>
-      <c r="G179">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="3">
-        <v>44695</v>
-      </c>
-      <c r="B180" s="4">
-        <v>6474.39</v>
-      </c>
-      <c r="C180" s="4">
-        <v>4850.71</v>
-      </c>
-      <c r="D180" s="4">
-        <v>1400.68</v>
-      </c>
-      <c r="E180" s="4">
-        <v>223</v>
-      </c>
-      <c r="F180" s="4">
-        <v>3760.14</v>
-      </c>
-      <c r="G180">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="3">
-        <v>44696</v>
-      </c>
-      <c r="B181" s="4">
-        <v>2278.7600000000002</v>
-      </c>
-      <c r="C181" s="4">
-        <v>2011.17</v>
-      </c>
-      <c r="D181" s="4">
-        <v>267.58999999999997</v>
-      </c>
-      <c r="E181" s="4">
-        <v>0</v>
-      </c>
-      <c r="F181" s="4">
-        <v>1349.34</v>
-      </c>
-      <c r="G181">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="3">
-        <v>44709</v>
-      </c>
-      <c r="B182" s="4">
-        <v>3786.59</v>
-      </c>
-      <c r="C182" s="4">
-        <v>3228.34</v>
-      </c>
-      <c r="D182" s="4">
-        <v>376.56</v>
-      </c>
-      <c r="E182" s="4">
-        <v>181.69</v>
-      </c>
-      <c r="F182" s="4">
-        <v>2274.87</v>
-      </c>
-      <c r="G182">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="3">
-        <v>44710</v>
-      </c>
-      <c r="B183" s="4">
-        <v>3963.06</v>
-      </c>
-      <c r="C183" s="4">
-        <v>3963.06</v>
-      </c>
-      <c r="D183" s="4">
-        <v>0</v>
-      </c>
-      <c r="E183" s="4">
-        <v>0</v>
-      </c>
-      <c r="F183" s="4">
-        <v>2283.02</v>
-      </c>
-      <c r="G183">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="3">
-        <v>44618</v>
-      </c>
-      <c r="B184" s="4">
-        <v>7506.01</v>
-      </c>
-      <c r="C184" s="4">
-        <v>4240.6499999999996</v>
-      </c>
-      <c r="D184" s="4">
-        <v>3265.36</v>
-      </c>
-      <c r="E184" s="4">
-        <v>0</v>
-      </c>
-      <c r="F184" s="4">
-        <v>4222.74</v>
-      </c>
-      <c r="G184">
-        <v>49</v>
-      </c>
-    </row>
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="C160"/>
+      <c r="D160"/>
+      <c r="E160"/>
+      <c r="F160"/>
+    </row>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5469,7 +4821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF169ED-0A5B-4E85-A1DC-CF4116D4BB32}">
   <dimension ref="B2:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat: Agrega clase 2 de Excel
</commit_message>
<xml_diff>
--- a/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
+++ b/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\codev\dev\projects\learning\data-analyst\excel-intermedio-tableros-formulas\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA808DB-996E-47C4-9626-B5DED0B9DF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87AB294-16D8-4E38-BBC3-BB8016CBD78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" firstSheet="3" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ventas" sheetId="3" r:id="rId1"/>
@@ -286,7 +286,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +297,7 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -668,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C0ADA3-4C22-4CF9-8AD3-3A127D5F6CB1}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G184"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4264,6 +4265,15 @@
     <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="B2:B152">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="2000"/>
+        <cfvo type="num" val="3000"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4272,38 +4282,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A23CDF-F090-4714-AB49-78B50071C889}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4320,19 +4333,19 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8">
         <v>28333.934600000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>21584.245800000001</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="8">
         <v>24285.437999999998</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="8">
         <v>22525.869900000002</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="8">
         <v>27973.243200000001</v>
       </c>
     </row>
@@ -4349,19 +4362,19 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="8">
         <v>14782.922399999999</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>19923.9192</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="8">
         <v>26713.981800000001</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
         <v>20154.725699999999</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="8">
         <v>26641.184000000001</v>
       </c>
     </row>
@@ -4378,19 +4391,19 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>27102.024399999998</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>25458.341199999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>23071.166099999999</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>23711.441999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="8">
         <v>30637.3616</v>
       </c>
     </row>
@@ -4407,19 +4420,19 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>22174.383600000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <v>23244.572400000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="8">
         <v>20642.622299999999</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>24897.0141</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="8">
         <v>25309.124800000001</v>
       </c>
     </row>
@@ -4436,23 +4449,35 @@
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8">
         <v>30797.755000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <v>20477.361400000002</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="8">
         <v>26713.981800000001</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <v>27268.158299999999</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="8">
         <v>22645.006399999998</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:I6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF002060"/>
+        <color theme="8"/>
+        <color theme="8" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Feat: Agrega clase sobre tablas dinamicas
</commit_message>
<xml_diff>
--- a/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
+++ b/data-analyst/excel-intermedio-tableros-formulas/recursos/ventas.xlsx
@@ -8,25 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\codev\dev\projects\learning\data-analyst\excel-intermedio-tableros-formulas\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87AB294-16D8-4E38-BBC3-BB8016CBD78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A0A39C-45D2-4E31-9790-87301A8585A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4E16050-6D6A-49A1-83DA-C4CBD7B8666B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ventas" sheetId="3" r:id="rId1"/>
-    <sheet name="Ventas x vendedor" sheetId="5" r:id="rId2"/>
-    <sheet name="Ventas x tienda" sheetId="6" r:id="rId3"/>
-    <sheet name="Gastos mensuales" sheetId="7" r:id="rId4"/>
-    <sheet name="Registro clientes" sheetId="8" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId1"/>
+    <sheet name="Ventas" sheetId="3" r:id="rId2"/>
+    <sheet name="Ventas x vendedor" sheetId="5" r:id="rId3"/>
+    <sheet name="Ventas x tienda" sheetId="6" r:id="rId4"/>
+    <sheet name="Gastos mensuales" sheetId="7" r:id="rId5"/>
+    <sheet name="Registro clientes" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ventas!$A$1:$A$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ventas!$A$1:$A$163</definedName>
     <definedName name="JR_PAGE_ANCHOR_0_1">[1]Ventas!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId8"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Vendedor</t>
   </si>
@@ -206,6 +210,36 @@
   <si>
     <t>Mantenimiento</t>
   </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Suma de Ventas totales</t>
+  </si>
+  <si>
+    <t>% ventas</t>
+  </si>
+  <si>
+    <t>Promedio de Tickets</t>
+  </si>
 </sst>
 </file>
 
@@ -286,7 +320,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,13 +332,66 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{8F53062A-67EE-41F0-AC5B-03CBEEF10C8A}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -368,6 +455,2581 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Cristian F. Orrego D." refreshedDate="45768.665600115739" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="151" xr:uid="{F9EB38A4-7B20-4492-8E6E-9CF9002051E0}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G152" sheet="Ventas"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="Fecha" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-01-01T00:00:00" maxDate="2022-06-01T00:00:00" count="151">
+        <d v="2022-01-01T00:00:00"/>
+        <d v="2022-01-02T00:00:00"/>
+        <d v="2022-01-03T00:00:00"/>
+        <d v="2022-01-04T00:00:00"/>
+        <d v="2022-01-05T00:00:00"/>
+        <d v="2022-01-06T00:00:00"/>
+        <d v="2022-01-07T00:00:00"/>
+        <d v="2022-01-08T00:00:00"/>
+        <d v="2022-01-09T00:00:00"/>
+        <d v="2022-01-10T00:00:00"/>
+        <d v="2022-01-11T00:00:00"/>
+        <d v="2022-01-12T00:00:00"/>
+        <d v="2022-01-13T00:00:00"/>
+        <d v="2022-01-14T00:00:00"/>
+        <d v="2022-01-15T00:00:00"/>
+        <d v="2022-01-16T00:00:00"/>
+        <d v="2022-01-17T00:00:00"/>
+        <d v="2022-01-18T00:00:00"/>
+        <d v="2022-01-19T00:00:00"/>
+        <d v="2022-01-20T00:00:00"/>
+        <d v="2022-01-21T00:00:00"/>
+        <d v="2022-01-22T00:00:00"/>
+        <d v="2022-01-23T00:00:00"/>
+        <d v="2022-01-24T00:00:00"/>
+        <d v="2022-01-25T00:00:00"/>
+        <d v="2022-01-26T00:00:00"/>
+        <d v="2022-01-27T00:00:00"/>
+        <d v="2022-01-28T00:00:00"/>
+        <d v="2022-01-29T00:00:00"/>
+        <d v="2022-01-30T00:00:00"/>
+        <d v="2022-01-31T00:00:00"/>
+        <d v="2022-02-01T00:00:00"/>
+        <d v="2022-02-02T00:00:00"/>
+        <d v="2022-02-03T00:00:00"/>
+        <d v="2022-02-04T00:00:00"/>
+        <d v="2022-02-05T00:00:00"/>
+        <d v="2022-02-06T00:00:00"/>
+        <d v="2022-02-07T00:00:00"/>
+        <d v="2022-02-08T00:00:00"/>
+        <d v="2022-02-09T00:00:00"/>
+        <d v="2022-02-10T00:00:00"/>
+        <d v="2022-02-11T00:00:00"/>
+        <d v="2022-02-12T00:00:00"/>
+        <d v="2022-02-13T00:00:00"/>
+        <d v="2022-02-14T00:00:00"/>
+        <d v="2022-02-15T00:00:00"/>
+        <d v="2022-02-16T00:00:00"/>
+        <d v="2022-02-17T00:00:00"/>
+        <d v="2022-02-18T00:00:00"/>
+        <d v="2022-02-19T00:00:00"/>
+        <d v="2022-02-20T00:00:00"/>
+        <d v="2022-02-21T00:00:00"/>
+        <d v="2022-02-22T00:00:00"/>
+        <d v="2022-02-23T00:00:00"/>
+        <d v="2022-02-24T00:00:00"/>
+        <d v="2022-02-25T00:00:00"/>
+        <d v="2022-02-26T00:00:00"/>
+        <d v="2022-02-27T00:00:00"/>
+        <d v="2022-02-28T00:00:00"/>
+        <d v="2022-03-01T00:00:00"/>
+        <d v="2022-03-02T00:00:00"/>
+        <d v="2022-03-03T00:00:00"/>
+        <d v="2022-03-04T00:00:00"/>
+        <d v="2022-03-05T00:00:00"/>
+        <d v="2022-03-06T00:00:00"/>
+        <d v="2022-03-07T00:00:00"/>
+        <d v="2022-03-08T00:00:00"/>
+        <d v="2022-03-09T00:00:00"/>
+        <d v="2022-03-10T00:00:00"/>
+        <d v="2022-03-11T00:00:00"/>
+        <d v="2022-03-12T00:00:00"/>
+        <d v="2022-03-13T00:00:00"/>
+        <d v="2022-03-14T00:00:00"/>
+        <d v="2022-03-15T00:00:00"/>
+        <d v="2022-03-16T00:00:00"/>
+        <d v="2022-03-17T00:00:00"/>
+        <d v="2022-03-18T00:00:00"/>
+        <d v="2022-03-19T00:00:00"/>
+        <d v="2022-03-20T00:00:00"/>
+        <d v="2022-03-21T00:00:00"/>
+        <d v="2022-03-22T00:00:00"/>
+        <d v="2022-03-23T00:00:00"/>
+        <d v="2022-03-24T00:00:00"/>
+        <d v="2022-03-25T00:00:00"/>
+        <d v="2022-03-26T00:00:00"/>
+        <d v="2022-03-27T00:00:00"/>
+        <d v="2022-03-28T00:00:00"/>
+        <d v="2022-03-29T00:00:00"/>
+        <d v="2022-03-30T00:00:00"/>
+        <d v="2022-03-31T00:00:00"/>
+        <d v="2022-04-01T00:00:00"/>
+        <d v="2022-04-02T00:00:00"/>
+        <d v="2022-04-03T00:00:00"/>
+        <d v="2022-04-04T00:00:00"/>
+        <d v="2022-04-05T00:00:00"/>
+        <d v="2022-04-06T00:00:00"/>
+        <d v="2022-04-07T00:00:00"/>
+        <d v="2022-04-08T00:00:00"/>
+        <d v="2022-04-09T00:00:00"/>
+        <d v="2022-04-10T00:00:00"/>
+        <d v="2022-04-11T00:00:00"/>
+        <d v="2022-04-12T00:00:00"/>
+        <d v="2022-04-13T00:00:00"/>
+        <d v="2022-04-14T00:00:00"/>
+        <d v="2022-04-15T00:00:00"/>
+        <d v="2022-04-16T00:00:00"/>
+        <d v="2022-04-17T00:00:00"/>
+        <d v="2022-04-18T00:00:00"/>
+        <d v="2022-04-19T00:00:00"/>
+        <d v="2022-04-20T00:00:00"/>
+        <d v="2022-04-21T00:00:00"/>
+        <d v="2022-04-22T00:00:00"/>
+        <d v="2022-04-23T00:00:00"/>
+        <d v="2022-04-24T00:00:00"/>
+        <d v="2022-04-25T00:00:00"/>
+        <d v="2022-04-26T00:00:00"/>
+        <d v="2022-04-27T00:00:00"/>
+        <d v="2022-04-28T00:00:00"/>
+        <d v="2022-04-29T00:00:00"/>
+        <d v="2022-04-30T00:00:00"/>
+        <d v="2022-05-01T00:00:00"/>
+        <d v="2022-05-02T00:00:00"/>
+        <d v="2022-05-03T00:00:00"/>
+        <d v="2022-05-04T00:00:00"/>
+        <d v="2022-05-05T00:00:00"/>
+        <d v="2022-05-06T00:00:00"/>
+        <d v="2022-05-07T00:00:00"/>
+        <d v="2022-05-08T00:00:00"/>
+        <d v="2022-05-09T00:00:00"/>
+        <d v="2022-05-10T00:00:00"/>
+        <d v="2022-05-11T00:00:00"/>
+        <d v="2022-05-12T00:00:00"/>
+        <d v="2022-05-13T00:00:00"/>
+        <d v="2022-05-14T00:00:00"/>
+        <d v="2022-05-15T00:00:00"/>
+        <d v="2022-05-16T00:00:00"/>
+        <d v="2022-05-17T00:00:00"/>
+        <d v="2022-05-18T00:00:00"/>
+        <d v="2022-05-19T00:00:00"/>
+        <d v="2022-05-20T00:00:00"/>
+        <d v="2022-05-21T00:00:00"/>
+        <d v="2022-05-22T00:00:00"/>
+        <d v="2022-05-23T00:00:00"/>
+        <d v="2022-05-24T00:00:00"/>
+        <d v="2022-05-25T00:00:00"/>
+        <d v="2022-05-26T00:00:00"/>
+        <d v="2022-05-27T00:00:00"/>
+        <d v="2022-05-28T00:00:00"/>
+        <d v="2022-05-29T00:00:00"/>
+        <d v="2022-05-30T00:00:00"/>
+        <d v="2022-05-31T00:00:00"/>
+      </sharedItems>
+      <fieldGroup par="8"/>
+    </cacheField>
+    <cacheField name="Ventas totales" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="10255.379999999999"/>
+    </cacheField>
+    <cacheField name="Ventas efectivo" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="8344.65"/>
+    </cacheField>
+    <cacheField name="Ventas tarjeta" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="3265.36"/>
+    </cacheField>
+    <cacheField name="Ventas transferencia" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="5132.3599999999997"/>
+    </cacheField>
+    <cacheField name="Utilidad" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="6062.86"/>
+    </cacheField>
+    <cacheField name="Tickets" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="73"/>
+    </cacheField>
+    <cacheField name="Días (Fecha)" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="days" startDate="2022-01-01T00:00:00" endDate="2022-06-01T00:00:00"/>
+        <groupItems count="368">
+          <s v="&lt;1/1/2022"/>
+          <s v="1-Jan"/>
+          <s v="2-Jan"/>
+          <s v="3-Jan"/>
+          <s v="4-Jan"/>
+          <s v="5-Jan"/>
+          <s v="6-Jan"/>
+          <s v="7-Jan"/>
+          <s v="8-Jan"/>
+          <s v="9-Jan"/>
+          <s v="10-Jan"/>
+          <s v="11-Jan"/>
+          <s v="12-Jan"/>
+          <s v="13-Jan"/>
+          <s v="14-Jan"/>
+          <s v="15-Jan"/>
+          <s v="16-Jan"/>
+          <s v="17-Jan"/>
+          <s v="18-Jan"/>
+          <s v="19-Jan"/>
+          <s v="20-Jan"/>
+          <s v="21-Jan"/>
+          <s v="22-Jan"/>
+          <s v="23-Jan"/>
+          <s v="24-Jan"/>
+          <s v="25-Jan"/>
+          <s v="26-Jan"/>
+          <s v="27-Jan"/>
+          <s v="28-Jan"/>
+          <s v="29-Jan"/>
+          <s v="30-Jan"/>
+          <s v="31-Jan"/>
+          <s v="1-Feb"/>
+          <s v="2-Feb"/>
+          <s v="3-Feb"/>
+          <s v="4-Feb"/>
+          <s v="5-Feb"/>
+          <s v="6-Feb"/>
+          <s v="7-Feb"/>
+          <s v="8-Feb"/>
+          <s v="9-Feb"/>
+          <s v="10-Feb"/>
+          <s v="11-Feb"/>
+          <s v="12-Feb"/>
+          <s v="13-Feb"/>
+          <s v="14-Feb"/>
+          <s v="15-Feb"/>
+          <s v="16-Feb"/>
+          <s v="17-Feb"/>
+          <s v="18-Feb"/>
+          <s v="19-Feb"/>
+          <s v="20-Feb"/>
+          <s v="21-Feb"/>
+          <s v="22-Feb"/>
+          <s v="23-Feb"/>
+          <s v="24-Feb"/>
+          <s v="25-Feb"/>
+          <s v="26-Feb"/>
+          <s v="27-Feb"/>
+          <s v="28-Feb"/>
+          <s v="29-Feb"/>
+          <s v="1-Mar"/>
+          <s v="2-Mar"/>
+          <s v="3-Mar"/>
+          <s v="4-Mar"/>
+          <s v="5-Mar"/>
+          <s v="6-Mar"/>
+          <s v="7-Mar"/>
+          <s v="8-Mar"/>
+          <s v="9-Mar"/>
+          <s v="10-Mar"/>
+          <s v="11-Mar"/>
+          <s v="12-Mar"/>
+          <s v="13-Mar"/>
+          <s v="14-Mar"/>
+          <s v="15-Mar"/>
+          <s v="16-Mar"/>
+          <s v="17-Mar"/>
+          <s v="18-Mar"/>
+          <s v="19-Mar"/>
+          <s v="20-Mar"/>
+          <s v="21-Mar"/>
+          <s v="22-Mar"/>
+          <s v="23-Mar"/>
+          <s v="24-Mar"/>
+          <s v="25-Mar"/>
+          <s v="26-Mar"/>
+          <s v="27-Mar"/>
+          <s v="28-Mar"/>
+          <s v="29-Mar"/>
+          <s v="30-Mar"/>
+          <s v="31-Mar"/>
+          <s v="1-Apr"/>
+          <s v="2-Apr"/>
+          <s v="3-Apr"/>
+          <s v="4-Apr"/>
+          <s v="5-Apr"/>
+          <s v="6-Apr"/>
+          <s v="7-Apr"/>
+          <s v="8-Apr"/>
+          <s v="9-Apr"/>
+          <s v="10-Apr"/>
+          <s v="11-Apr"/>
+          <s v="12-Apr"/>
+          <s v="13-Apr"/>
+          <s v="14-Apr"/>
+          <s v="15-Apr"/>
+          <s v="16-Apr"/>
+          <s v="17-Apr"/>
+          <s v="18-Apr"/>
+          <s v="19-Apr"/>
+          <s v="20-Apr"/>
+          <s v="21-Apr"/>
+          <s v="22-Apr"/>
+          <s v="23-Apr"/>
+          <s v="24-Apr"/>
+          <s v="25-Apr"/>
+          <s v="26-Apr"/>
+          <s v="27-Apr"/>
+          <s v="28-Apr"/>
+          <s v="29-Apr"/>
+          <s v="30-Apr"/>
+          <s v="1-May"/>
+          <s v="2-May"/>
+          <s v="3-May"/>
+          <s v="4-May"/>
+          <s v="5-May"/>
+          <s v="6-May"/>
+          <s v="7-May"/>
+          <s v="8-May"/>
+          <s v="9-May"/>
+          <s v="10-May"/>
+          <s v="11-May"/>
+          <s v="12-May"/>
+          <s v="13-May"/>
+          <s v="14-May"/>
+          <s v="15-May"/>
+          <s v="16-May"/>
+          <s v="17-May"/>
+          <s v="18-May"/>
+          <s v="19-May"/>
+          <s v="20-May"/>
+          <s v="21-May"/>
+          <s v="22-May"/>
+          <s v="23-May"/>
+          <s v="24-May"/>
+          <s v="25-May"/>
+          <s v="26-May"/>
+          <s v="27-May"/>
+          <s v="28-May"/>
+          <s v="29-May"/>
+          <s v="30-May"/>
+          <s v="31-May"/>
+          <s v="1-Jun"/>
+          <s v="2-Jun"/>
+          <s v="3-Jun"/>
+          <s v="4-Jun"/>
+          <s v="5-Jun"/>
+          <s v="6-Jun"/>
+          <s v="7-Jun"/>
+          <s v="8-Jun"/>
+          <s v="9-Jun"/>
+          <s v="10-Jun"/>
+          <s v="11-Jun"/>
+          <s v="12-Jun"/>
+          <s v="13-Jun"/>
+          <s v="14-Jun"/>
+          <s v="15-Jun"/>
+          <s v="16-Jun"/>
+          <s v="17-Jun"/>
+          <s v="18-Jun"/>
+          <s v="19-Jun"/>
+          <s v="20-Jun"/>
+          <s v="21-Jun"/>
+          <s v="22-Jun"/>
+          <s v="23-Jun"/>
+          <s v="24-Jun"/>
+          <s v="25-Jun"/>
+          <s v="26-Jun"/>
+          <s v="27-Jun"/>
+          <s v="28-Jun"/>
+          <s v="29-Jun"/>
+          <s v="30-Jun"/>
+          <s v="1-Jul"/>
+          <s v="2-Jul"/>
+          <s v="3-Jul"/>
+          <s v="4-Jul"/>
+          <s v="5-Jul"/>
+          <s v="6-Jul"/>
+          <s v="7-Jul"/>
+          <s v="8-Jul"/>
+          <s v="9-Jul"/>
+          <s v="10-Jul"/>
+          <s v="11-Jul"/>
+          <s v="12-Jul"/>
+          <s v="13-Jul"/>
+          <s v="14-Jul"/>
+          <s v="15-Jul"/>
+          <s v="16-Jul"/>
+          <s v="17-Jul"/>
+          <s v="18-Jul"/>
+          <s v="19-Jul"/>
+          <s v="20-Jul"/>
+          <s v="21-Jul"/>
+          <s v="22-Jul"/>
+          <s v="23-Jul"/>
+          <s v="24-Jul"/>
+          <s v="25-Jul"/>
+          <s v="26-Jul"/>
+          <s v="27-Jul"/>
+          <s v="28-Jul"/>
+          <s v="29-Jul"/>
+          <s v="30-Jul"/>
+          <s v="31-Jul"/>
+          <s v="1-Aug"/>
+          <s v="2-Aug"/>
+          <s v="3-Aug"/>
+          <s v="4-Aug"/>
+          <s v="5-Aug"/>
+          <s v="6-Aug"/>
+          <s v="7-Aug"/>
+          <s v="8-Aug"/>
+          <s v="9-Aug"/>
+          <s v="10-Aug"/>
+          <s v="11-Aug"/>
+          <s v="12-Aug"/>
+          <s v="13-Aug"/>
+          <s v="14-Aug"/>
+          <s v="15-Aug"/>
+          <s v="16-Aug"/>
+          <s v="17-Aug"/>
+          <s v="18-Aug"/>
+          <s v="19-Aug"/>
+          <s v="20-Aug"/>
+          <s v="21-Aug"/>
+          <s v="22-Aug"/>
+          <s v="23-Aug"/>
+          <s v="24-Aug"/>
+          <s v="25-Aug"/>
+          <s v="26-Aug"/>
+          <s v="27-Aug"/>
+          <s v="28-Aug"/>
+          <s v="29-Aug"/>
+          <s v="30-Aug"/>
+          <s v="31-Aug"/>
+          <s v="1-Sep"/>
+          <s v="2-Sep"/>
+          <s v="3-Sep"/>
+          <s v="4-Sep"/>
+          <s v="5-Sep"/>
+          <s v="6-Sep"/>
+          <s v="7-Sep"/>
+          <s v="8-Sep"/>
+          <s v="9-Sep"/>
+          <s v="10-Sep"/>
+          <s v="11-Sep"/>
+          <s v="12-Sep"/>
+          <s v="13-Sep"/>
+          <s v="14-Sep"/>
+          <s v="15-Sep"/>
+          <s v="16-Sep"/>
+          <s v="17-Sep"/>
+          <s v="18-Sep"/>
+          <s v="19-Sep"/>
+          <s v="20-Sep"/>
+          <s v="21-Sep"/>
+          <s v="22-Sep"/>
+          <s v="23-Sep"/>
+          <s v="24-Sep"/>
+          <s v="25-Sep"/>
+          <s v="26-Sep"/>
+          <s v="27-Sep"/>
+          <s v="28-Sep"/>
+          <s v="29-Sep"/>
+          <s v="30-Sep"/>
+          <s v="1-Oct"/>
+          <s v="2-Oct"/>
+          <s v="3-Oct"/>
+          <s v="4-Oct"/>
+          <s v="5-Oct"/>
+          <s v="6-Oct"/>
+          <s v="7-Oct"/>
+          <s v="8-Oct"/>
+          <s v="9-Oct"/>
+          <s v="10-Oct"/>
+          <s v="11-Oct"/>
+          <s v="12-Oct"/>
+          <s v="13-Oct"/>
+          <s v="14-Oct"/>
+          <s v="15-Oct"/>
+          <s v="16-Oct"/>
+          <s v="17-Oct"/>
+          <s v="18-Oct"/>
+          <s v="19-Oct"/>
+          <s v="20-Oct"/>
+          <s v="21-Oct"/>
+          <s v="22-Oct"/>
+          <s v="23-Oct"/>
+          <s v="24-Oct"/>
+          <s v="25-Oct"/>
+          <s v="26-Oct"/>
+          <s v="27-Oct"/>
+          <s v="28-Oct"/>
+          <s v="29-Oct"/>
+          <s v="30-Oct"/>
+          <s v="31-Oct"/>
+          <s v="1-Nov"/>
+          <s v="2-Nov"/>
+          <s v="3-Nov"/>
+          <s v="4-Nov"/>
+          <s v="5-Nov"/>
+          <s v="6-Nov"/>
+          <s v="7-Nov"/>
+          <s v="8-Nov"/>
+          <s v="9-Nov"/>
+          <s v="10-Nov"/>
+          <s v="11-Nov"/>
+          <s v="12-Nov"/>
+          <s v="13-Nov"/>
+          <s v="14-Nov"/>
+          <s v="15-Nov"/>
+          <s v="16-Nov"/>
+          <s v="17-Nov"/>
+          <s v="18-Nov"/>
+          <s v="19-Nov"/>
+          <s v="20-Nov"/>
+          <s v="21-Nov"/>
+          <s v="22-Nov"/>
+          <s v="23-Nov"/>
+          <s v="24-Nov"/>
+          <s v="25-Nov"/>
+          <s v="26-Nov"/>
+          <s v="27-Nov"/>
+          <s v="28-Nov"/>
+          <s v="29-Nov"/>
+          <s v="30-Nov"/>
+          <s v="1-Dec"/>
+          <s v="2-Dec"/>
+          <s v="3-Dec"/>
+          <s v="4-Dec"/>
+          <s v="5-Dec"/>
+          <s v="6-Dec"/>
+          <s v="7-Dec"/>
+          <s v="8-Dec"/>
+          <s v="9-Dec"/>
+          <s v="10-Dec"/>
+          <s v="11-Dec"/>
+          <s v="12-Dec"/>
+          <s v="13-Dec"/>
+          <s v="14-Dec"/>
+          <s v="15-Dec"/>
+          <s v="16-Dec"/>
+          <s v="17-Dec"/>
+          <s v="18-Dec"/>
+          <s v="19-Dec"/>
+          <s v="20-Dec"/>
+          <s v="21-Dec"/>
+          <s v="22-Dec"/>
+          <s v="23-Dec"/>
+          <s v="24-Dec"/>
+          <s v="25-Dec"/>
+          <s v="26-Dec"/>
+          <s v="27-Dec"/>
+          <s v="28-Dec"/>
+          <s v="29-Dec"/>
+          <s v="30-Dec"/>
+          <s v="31-Dec"/>
+          <s v="&gt;6/1/2022"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Meses (Fecha)" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="months" startDate="2022-01-01T00:00:00" endDate="2022-06-01T00:00:00"/>
+        <groupItems count="14">
+          <s v="&lt;1/1/2022"/>
+          <s v="Jan"/>
+          <s v="Feb"/>
+          <s v="Mar"/>
+          <s v="Apr"/>
+          <s v="May"/>
+          <s v="Jun"/>
+          <s v="Jul"/>
+          <s v="Aug"/>
+          <s v="Sep"/>
+          <s v="Oct"/>
+          <s v="Nov"/>
+          <s v="Dec"/>
+          <s v="&gt;6/1/2022"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="151">
+  <r>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3574.28"/>
+    <n v="3459.57"/>
+    <n v="114.71"/>
+    <n v="0"/>
+    <n v="1908.81"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4942.17"/>
+    <n v="4942.17"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2553.7800000000002"/>
+    <n v="47"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="5551.82"/>
+    <n v="5108.04"/>
+    <n v="443.78"/>
+    <n v="0"/>
+    <n v="2692.46"/>
+    <n v="55"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="6001.55"/>
+    <n v="5876.3"/>
+    <n v="125.25"/>
+    <n v="0"/>
+    <n v="3018.65"/>
+    <n v="58"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="4118.8900000000003"/>
+    <n v="3962.21"/>
+    <n v="156.68"/>
+    <n v="0"/>
+    <n v="2053.39"/>
+    <n v="50"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="5649.31"/>
+    <n v="4933.16"/>
+    <n v="716.15"/>
+    <n v="0"/>
+    <n v="2779.85"/>
+    <n v="59"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="5302.13"/>
+    <n v="4907.66"/>
+    <n v="394.47"/>
+    <n v="0"/>
+    <n v="2587.8000000000002"/>
+    <n v="58"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3478.01"/>
+    <n v="1596.41"/>
+    <n v="1881.6"/>
+    <n v="0"/>
+    <n v="1746.17"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="7573.72"/>
+    <n v="2347.08"/>
+    <n v="94.28"/>
+    <n v="5132.3599999999997"/>
+    <n v="3802.33"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="4226.25"/>
+    <n v="3692.89"/>
+    <n v="533.36"/>
+    <n v="0"/>
+    <n v="2411.77"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="4172.46"/>
+    <n v="4172.46"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2291.9499999999998"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3580.9"/>
+    <n v="3217.79"/>
+    <n v="363.11"/>
+    <n v="0"/>
+    <n v="2032.93"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3503.12"/>
+    <n v="2831.55"/>
+    <n v="671.57"/>
+    <n v="0"/>
+    <n v="1996.33"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="6727.53"/>
+    <n v="5752.18"/>
+    <n v="975.35"/>
+    <n v="0"/>
+    <n v="3750.84"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3620.16"/>
+    <n v="3216.57"/>
+    <n v="403.59"/>
+    <n v="0"/>
+    <n v="2127.77"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3178.41"/>
+    <n v="3154.41"/>
+    <n v="24"/>
+    <n v="0"/>
+    <n v="1826.18"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3765.94"/>
+    <n v="3388.37"/>
+    <n v="377.57"/>
+    <n v="0"/>
+    <n v="2082.56"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="3966.48"/>
+    <n v="3605.21"/>
+    <n v="361.27"/>
+    <n v="0"/>
+    <n v="2216.8200000000002"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3706.63"/>
+    <n v="3706.63"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2076.33"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="2753.61"/>
+    <n v="2753.61"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1611.89"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="6177.15"/>
+    <n v="4991.5600000000004"/>
+    <n v="1185.5899999999999"/>
+    <n v="0"/>
+    <n v="3505.85"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="2919.39"/>
+    <n v="2833.64"/>
+    <n v="85.75"/>
+    <n v="0"/>
+    <n v="1654.02"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3034.94"/>
+    <n v="2721.46"/>
+    <n v="313.48"/>
+    <n v="0"/>
+    <n v="1758.41"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <n v="2491.39"/>
+    <n v="2365.77"/>
+    <n v="125.62"/>
+    <n v="0"/>
+    <n v="1430.55"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <n v="1881.23"/>
+    <n v="1714.15"/>
+    <n v="167.08"/>
+    <n v="0"/>
+    <n v="1141.31"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <n v="2533.27"/>
+    <n v="1714.63"/>
+    <n v="818.64"/>
+    <n v="0"/>
+    <n v="1442.5"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <n v="4445.8599999999997"/>
+    <n v="4286.07"/>
+    <n v="159.79"/>
+    <n v="0"/>
+    <n v="2488.38"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <n v="3152.18"/>
+    <n v="2150.65"/>
+    <n v="1001.53"/>
+    <n v="0"/>
+    <n v="1844.08"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <n v="2940.98"/>
+    <n v="2819.89"/>
+    <n v="121.09"/>
+    <n v="0"/>
+    <n v="1669.58"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <n v="4221.26"/>
+    <n v="4169.25"/>
+    <n v="52.01"/>
+    <n v="0"/>
+    <n v="2391.35"/>
+    <n v="54"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <n v="4717.8500000000004"/>
+    <n v="4360.6400000000003"/>
+    <n v="357.21"/>
+    <n v="0"/>
+    <n v="2616.06"/>
+    <n v="47"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <n v="4845.28"/>
+    <n v="4845.28"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2699.69"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <n v="3418.45"/>
+    <n v="3305.74"/>
+    <n v="112.71"/>
+    <n v="0"/>
+    <n v="1962.65"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <n v="3483.92"/>
+    <n v="2786.75"/>
+    <n v="697.17"/>
+    <n v="0"/>
+    <n v="1975.94"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <n v="4180.18"/>
+    <n v="3462.69"/>
+    <n v="717.49"/>
+    <n v="0"/>
+    <n v="2371.66"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <n v="2630.46"/>
+    <n v="1803.43"/>
+    <n v="827.03"/>
+    <n v="0"/>
+    <n v="1669.58"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <n v="2654.27"/>
+    <n v="2012.41"/>
+    <n v="641.86"/>
+    <n v="0"/>
+    <n v="1524.11"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <n v="1405.34"/>
+    <n v="1405.34"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="824.49"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <n v="3204.92"/>
+    <n v="2472.89"/>
+    <n v="732.03"/>
+    <n v="0"/>
+    <n v="1810.88"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <n v="3167.18"/>
+    <n v="2983.18"/>
+    <n v="184"/>
+    <n v="0"/>
+    <n v="1773.28"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <n v="2384.7800000000002"/>
+    <n v="2384.7800000000002"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1326.82"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <n v="4758.67"/>
+    <n v="4515.74"/>
+    <n v="242.93"/>
+    <n v="0"/>
+    <n v="2747.11"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <n v="2562.7199999999998"/>
+    <n v="2031.79"/>
+    <n v="530.92999999999995"/>
+    <n v="0"/>
+    <n v="1417.57"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <n v="2791.7"/>
+    <n v="2753.01"/>
+    <n v="38.69"/>
+    <n v="0"/>
+    <n v="1599.99"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <n v="6054.22"/>
+    <n v="5314.25"/>
+    <n v="739.97"/>
+    <n v="0"/>
+    <n v="3472.59"/>
+    <n v="56"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <n v="4255.83"/>
+    <n v="4245.07"/>
+    <n v="10.76"/>
+    <n v="0"/>
+    <n v="2387.1799999999998"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <n v="4820.66"/>
+    <n v="3842.05"/>
+    <n v="978.61"/>
+    <n v="0"/>
+    <n v="2765.3"/>
+    <n v="55"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <n v="2980.8"/>
+    <n v="2980.8"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1736.15"/>
+    <n v="37"/>
+  </r>
+  <r>
+    <x v="49"/>
+    <n v="5728.46"/>
+    <n v="4623.34"/>
+    <n v="1105.1199999999999"/>
+    <n v="0"/>
+    <n v="3210.62"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="50"/>
+    <n v="5559.94"/>
+    <n v="2744.5"/>
+    <n v="2815.44"/>
+    <n v="0"/>
+    <n v="1440.61"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="51"/>
+    <n v="4966.54"/>
+    <n v="4085.99"/>
+    <n v="880.55"/>
+    <n v="0"/>
+    <n v="2924.42"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="52"/>
+    <n v="4648.99"/>
+    <n v="4545.76"/>
+    <n v="103.23"/>
+    <n v="0"/>
+    <n v="2535.5100000000002"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <x v="53"/>
+    <n v="3440.66"/>
+    <n v="2997.29"/>
+    <n v="443.37"/>
+    <n v="0"/>
+    <n v="1976.46"/>
+    <n v="43"/>
+  </r>
+  <r>
+    <x v="54"/>
+    <n v="4088.09"/>
+    <n v="3492.17"/>
+    <n v="595.91999999999996"/>
+    <n v="0"/>
+    <n v="2317.0700000000002"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="55"/>
+    <n v="2918.34"/>
+    <n v="2489.85"/>
+    <n v="428.49"/>
+    <n v="0"/>
+    <n v="1668.94"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="56"/>
+    <n v="7506.01"/>
+    <n v="4240.6499999999996"/>
+    <n v="3265.36"/>
+    <n v="0"/>
+    <n v="4222.74"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <x v="57"/>
+    <n v="3184.52"/>
+    <n v="2716.03"/>
+    <n v="468.49"/>
+    <n v="0"/>
+    <n v="3015.9"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="58"/>
+    <n v="4329.66"/>
+    <n v="3982.75"/>
+    <n v="346.91"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="59"/>
+    <n v="6669.52"/>
+    <n v="5792.44"/>
+    <n v="877.08"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="60"/>
+  </r>
+  <r>
+    <x v="60"/>
+    <n v="2966.54"/>
+    <n v="2898.01"/>
+    <n v="68.53"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="61"/>
+    <n v="6080.77"/>
+    <n v="4636.5600000000004"/>
+    <n v="1444.21"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="50"/>
+  </r>
+  <r>
+    <x v="62"/>
+    <n v="3690.55"/>
+    <n v="3490.55"/>
+    <n v="200"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <x v="63"/>
+    <n v="5746.1"/>
+    <n v="4348.95"/>
+    <n v="1397.15"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="64"/>
+    <n v="3095.82"/>
+    <n v="2103.2800000000002"/>
+    <n v="992.54"/>
+    <n v="0"/>
+    <n v="1751.75"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="65"/>
+    <n v="3740.32"/>
+    <n v="3377.27"/>
+    <n v="363.05"/>
+    <n v="0"/>
+    <n v="2132.7800000000002"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="66"/>
+    <n v="5725.4"/>
+    <n v="4397.01"/>
+    <n v="1328.39"/>
+    <n v="0"/>
+    <n v="3161.2"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="67"/>
+    <n v="2361.6999999999998"/>
+    <n v="2361.6999999999998"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1436.16"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="68"/>
+    <n v="3606.48"/>
+    <n v="3297.16"/>
+    <n v="309.32"/>
+    <n v="0"/>
+    <n v="2165.2199999999998"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="69"/>
+    <n v="4566.46"/>
+    <n v="3666.12"/>
+    <n v="725.34"/>
+    <n v="175"/>
+    <n v="2708.65"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="70"/>
+    <n v="2883.33"/>
+    <n v="2424.5"/>
+    <n v="458.83"/>
+    <n v="0"/>
+    <n v="1764.21"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="71"/>
+    <n v="1853.87"/>
+    <n v="1323.77"/>
+    <n v="530.1"/>
+    <n v="0"/>
+    <n v="1137.25"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="72"/>
+    <n v="5483.77"/>
+    <n v="3538.24"/>
+    <n v="1945.53"/>
+    <n v="0"/>
+    <n v="3209.25"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="73"/>
+    <n v="5135.18"/>
+    <n v="4967.13"/>
+    <n v="168.05"/>
+    <n v="0"/>
+    <n v="3103.21"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="74"/>
+    <n v="3445.95"/>
+    <n v="3445.95"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2116.91"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="75"/>
+    <n v="4681.26"/>
+    <n v="3801.2"/>
+    <n v="880.06"/>
+    <n v="0"/>
+    <n v="2789.94"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="76"/>
+    <n v="4252.0200000000004"/>
+    <n v="3042.13"/>
+    <n v="1209.8900000000001"/>
+    <n v="0"/>
+    <n v="2512.66"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="77"/>
+    <n v="3686.54"/>
+    <n v="3434.56"/>
+    <n v="251.98"/>
+    <n v="0"/>
+    <n v="2280.5"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <x v="78"/>
+    <n v="3334.67"/>
+    <n v="2580.8000000000002"/>
+    <n v="753.87"/>
+    <n v="0"/>
+    <n v="2009.86"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="79"/>
+    <n v="3020.49"/>
+    <n v="3020.49"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1712.65"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="80"/>
+    <n v="1648.64"/>
+    <n v="1615.65"/>
+    <n v="32.99"/>
+    <n v="0"/>
+    <n v="1045.55"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="81"/>
+    <n v="2574.2399999999998"/>
+    <n v="2371.16"/>
+    <n v="203.08"/>
+    <n v="0"/>
+    <n v="1536.1"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="82"/>
+    <n v="2477.08"/>
+    <n v="2477.08"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1449.1"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="83"/>
+    <n v="4972.6000000000004"/>
+    <n v="4293.55"/>
+    <n v="679.05"/>
+    <n v="0"/>
+    <n v="3010.9"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="84"/>
+    <n v="5208.8999999999996"/>
+    <n v="4718.82"/>
+    <n v="490.08"/>
+    <n v="0"/>
+    <n v="3079.53"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="85"/>
+    <n v="1700.68"/>
+    <n v="1371.44"/>
+    <n v="329.24"/>
+    <n v="0"/>
+    <n v="996.19"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="86"/>
+    <n v="4589.2700000000004"/>
+    <n v="3800.38"/>
+    <n v="788.89"/>
+    <n v="0"/>
+    <n v="2821.77"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="87"/>
+    <n v="3952.03"/>
+    <n v="3196.76"/>
+    <n v="755.27"/>
+    <n v="0"/>
+    <n v="2391.38"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <x v="88"/>
+    <n v="2922.44"/>
+    <n v="2621.94"/>
+    <n v="300.5"/>
+    <n v="0"/>
+    <n v="1680.93"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="89"/>
+    <n v="5354.57"/>
+    <n v="4756.67"/>
+    <n v="597.9"/>
+    <n v="0"/>
+    <n v="3130.67"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="90"/>
+    <n v="10255.379999999999"/>
+    <n v="8344.65"/>
+    <n v="1910.73"/>
+    <n v="0"/>
+    <n v="6062.86"/>
+    <n v="73"/>
+  </r>
+  <r>
+    <x v="91"/>
+    <n v="3892.35"/>
+    <n v="3256.02"/>
+    <n v="636.33000000000004"/>
+    <n v="0"/>
+    <n v="2363.4"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="92"/>
+    <n v="1394.7"/>
+    <n v="1257.75"/>
+    <n v="136.94999999999999"/>
+    <n v="0"/>
+    <n v="849.14"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="93"/>
+    <n v="2904.19"/>
+    <n v="2723.13"/>
+    <n v="181.06"/>
+    <n v="0"/>
+    <n v="1778.45"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="94"/>
+    <n v="3574.76"/>
+    <n v="3106.79"/>
+    <n v="467.97"/>
+    <n v="0"/>
+    <n v="2169.77"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="95"/>
+    <n v="3552.24"/>
+    <n v="3143.27"/>
+    <n v="408.97"/>
+    <n v="0"/>
+    <n v="2140.11"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="96"/>
+    <n v="4385.3500000000004"/>
+    <n v="4385.3500000000004"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2619.86"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="97"/>
+    <n v="4999.97"/>
+    <n v="3970.51"/>
+    <n v="1029.46"/>
+    <n v="0"/>
+    <n v="2937.99"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <x v="98"/>
+    <n v="4886.8999999999996"/>
+    <n v="3893.99"/>
+    <n v="992.91"/>
+    <n v="0"/>
+    <n v="2862.35"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="99"/>
+    <n v="2396.5700000000002"/>
+    <n v="1637.17"/>
+    <n v="759.4"/>
+    <n v="0"/>
+    <n v="1412"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <x v="100"/>
+    <n v="3934.62"/>
+    <n v="3762.78"/>
+    <n v="171.84"/>
+    <n v="0"/>
+    <n v="2347.96"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="101"/>
+    <n v="7285.53"/>
+    <n v="6415.1"/>
+    <n v="870.43"/>
+    <n v="0"/>
+    <n v="4354.87"/>
+    <n v="61"/>
+  </r>
+  <r>
+    <x v="102"/>
+    <n v="7784.47"/>
+    <n v="7167.97"/>
+    <n v="616.5"/>
+    <n v="0"/>
+    <n v="4730.93"/>
+    <n v="66"/>
+  </r>
+  <r>
+    <x v="103"/>
+    <n v="2113.21"/>
+    <n v="1467.32"/>
+    <n v="645.89"/>
+    <n v="0"/>
+    <n v="1275.03"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="104"/>
+    <n v="2323.02"/>
+    <n v="2107.75"/>
+    <n v="215.27"/>
+    <n v="0"/>
+    <n v="1364.52"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="105"/>
+    <n v="2517.63"/>
+    <n v="1915.96"/>
+    <n v="601.66999999999996"/>
+    <n v="0"/>
+    <n v="1519.54"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="106"/>
+    <n v="3773.66"/>
+    <n v="3511.46"/>
+    <n v="262.2"/>
+    <n v="0"/>
+    <n v="2285.61"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="107"/>
+    <n v="4332.58"/>
+    <n v="3719.02"/>
+    <n v="613.55999999999995"/>
+    <n v="0"/>
+    <n v="2577.2800000000002"/>
+    <n v="47"/>
+  </r>
+  <r>
+    <x v="108"/>
+    <n v="4677.13"/>
+    <n v="4677.13"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2738.63"/>
+    <n v="57"/>
+  </r>
+  <r>
+    <x v="109"/>
+    <n v="7803.19"/>
+    <n v="7326.64"/>
+    <n v="476.55"/>
+    <n v="0"/>
+    <n v="4624.54"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="110"/>
+    <n v="4054.63"/>
+    <n v="3408.61"/>
+    <n v="646.02"/>
+    <n v="0"/>
+    <n v="2478.44"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="111"/>
+    <n v="3629.81"/>
+    <n v="3038.84"/>
+    <n v="590.97"/>
+    <n v="0"/>
+    <n v="2063.79"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="112"/>
+    <n v="2972.21"/>
+    <n v="2714.06"/>
+    <n v="258.14999999999998"/>
+    <n v="0"/>
+    <n v="1788.48"/>
+    <n v="37"/>
+  </r>
+  <r>
+    <x v="113"/>
+    <n v="1497.54"/>
+    <n v="1497.54"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="882.46"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="114"/>
+    <n v="3894.87"/>
+    <n v="3577.5"/>
+    <n v="317.37"/>
+    <n v="0"/>
+    <n v="2377.1"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="115"/>
+    <n v="2496.5700000000002"/>
+    <n v="2496.5700000000002"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="1464.89"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="116"/>
+    <n v="2155.31"/>
+    <n v="2126.83"/>
+    <n v="28.48"/>
+    <n v="0"/>
+    <n v="1304.44"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="117"/>
+    <n v="3407.9"/>
+    <n v="2741.14"/>
+    <n v="666.76"/>
+    <n v="0"/>
+    <n v="2015.66"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="118"/>
+    <n v="2724.02"/>
+    <n v="2616.0300000000002"/>
+    <n v="107.99"/>
+    <n v="0"/>
+    <n v="1600.48"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="119"/>
+    <n v="2936.9"/>
+    <n v="2120.46"/>
+    <n v="816.44"/>
+    <n v="0"/>
+    <n v="1733.86"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="120"/>
+    <n v="2299.4899999999998"/>
+    <n v="1844.27"/>
+    <n v="455.22"/>
+    <n v="0"/>
+    <n v="1358.02"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="121"/>
+    <n v="5005.97"/>
+    <n v="4914.97"/>
+    <n v="91"/>
+    <n v="0"/>
+    <n v="2991.38"/>
+    <n v="44"/>
+  </r>
+  <r>
+    <x v="122"/>
+    <n v="3559.06"/>
+    <n v="3026.82"/>
+    <n v="532.24"/>
+    <n v="0"/>
+    <n v="2125.69"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="123"/>
+    <n v="3769.1"/>
+    <n v="3769.1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2195.29"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="124"/>
+    <n v="4005.34"/>
+    <n v="3073.37"/>
+    <n v="931.97"/>
+    <n v="0"/>
+    <n v="2362.7600000000002"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="125"/>
+    <n v="3641.77"/>
+    <n v="3097.47"/>
+    <n v="544.29999999999995"/>
+    <n v="0"/>
+    <n v="2215.27"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="126"/>
+    <n v="3771.87"/>
+    <n v="3606.46"/>
+    <n v="165.41"/>
+    <n v="0"/>
+    <n v="2210.9"/>
+    <n v="37"/>
+  </r>
+  <r>
+    <x v="127"/>
+    <n v="4323.88"/>
+    <n v="4121.76"/>
+    <n v="202.12"/>
+    <n v="0"/>
+    <n v="2500.27"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="128"/>
+    <n v="6576.87"/>
+    <n v="4606.3999999999996"/>
+    <n v="1970.47"/>
+    <n v="0"/>
+    <n v="3815.44"/>
+    <n v="47"/>
+  </r>
+  <r>
+    <x v="129"/>
+    <n v="4187.87"/>
+    <n v="3274.09"/>
+    <n v="546.08000000000004"/>
+    <n v="367.7"/>
+    <n v="2428.3000000000002"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="130"/>
+    <n v="2697"/>
+    <n v="2265.39"/>
+    <n v="431.61"/>
+    <n v="0"/>
+    <n v="1614.29"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="131"/>
+    <n v="5016.97"/>
+    <n v="3192.75"/>
+    <n v="1824.22"/>
+    <n v="0"/>
+    <n v="2935.17"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="132"/>
+    <n v="6800.97"/>
+    <n v="5259.85"/>
+    <n v="1541.12"/>
+    <n v="0"/>
+    <n v="4028.82"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="133"/>
+    <n v="6474.39"/>
+    <n v="4850.71"/>
+    <n v="1400.68"/>
+    <n v="223"/>
+    <n v="3760.14"/>
+    <n v="45"/>
+  </r>
+  <r>
+    <x v="134"/>
+    <n v="2278.7600000000002"/>
+    <n v="2011.17"/>
+    <n v="267.58999999999997"/>
+    <n v="0"/>
+    <n v="1349.34"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="135"/>
+    <n v="6836.33"/>
+    <n v="5687.98"/>
+    <n v="1148.3499999999999"/>
+    <n v="0"/>
+    <n v="4091.26"/>
+    <n v="60"/>
+  </r>
+  <r>
+    <x v="136"/>
+    <n v="2978.96"/>
+    <n v="2784.96"/>
+    <n v="194"/>
+    <n v="0"/>
+    <n v="1801.97"/>
+    <n v="36"/>
+  </r>
+  <r>
+    <x v="137"/>
+    <n v="3994.34"/>
+    <n v="2886.69"/>
+    <n v="1107.6500000000001"/>
+    <n v="0"/>
+    <n v="2329.9499999999998"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="138"/>
+    <n v="3841.43"/>
+    <n v="3668.32"/>
+    <n v="173.11"/>
+    <n v="0"/>
+    <n v="2337.63"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="139"/>
+    <n v="5256.21"/>
+    <n v="4466.4799999999996"/>
+    <n v="318.81"/>
+    <n v="470.92"/>
+    <n v="3190.74"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="140"/>
+    <n v="4876.71"/>
+    <n v="4139.45"/>
+    <n v="737.26"/>
+    <n v="0"/>
+    <n v="2880.41"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="141"/>
+    <n v="3625.34"/>
+    <n v="2363.54"/>
+    <n v="1261.8"/>
+    <n v="0"/>
+    <n v="2172.88"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="142"/>
+    <n v="2353.56"/>
+    <n v="1970.94"/>
+    <n v="382.62"/>
+    <n v="0"/>
+    <n v="1398.95"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="143"/>
+    <n v="2837.77"/>
+    <n v="2560.34"/>
+    <n v="277.43"/>
+    <n v="0"/>
+    <n v="1671.61"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="144"/>
+    <n v="6485.35"/>
+    <n v="5601.1"/>
+    <n v="884.25"/>
+    <n v="0"/>
+    <n v="3843.54"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="145"/>
+    <n v="4079.26"/>
+    <n v="3574.25"/>
+    <n v="505.01"/>
+    <n v="0"/>
+    <n v="2365.6"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="146"/>
+    <n v="6378.39"/>
+    <n v="4568.8100000000004"/>
+    <n v="903.56"/>
+    <n v="906.02"/>
+    <n v="3894.37"/>
+    <n v="60"/>
+  </r>
+  <r>
+    <x v="147"/>
+    <n v="3786.59"/>
+    <n v="3228.34"/>
+    <n v="376.56"/>
+    <n v="181.69"/>
+    <n v="2274.87"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="148"/>
+    <n v="3963.06"/>
+    <n v="3963.06"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="2283.02"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="149"/>
+    <n v="4594.9449999999997"/>
+    <n v="3829.46"/>
+    <n v="765.48500000000001"/>
+    <n v="0"/>
+    <n v="2665.0681"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="150"/>
+    <n v="2908.3649999999998"/>
+    <n v="2672.65"/>
+    <n v="235.715"/>
+    <n v="0"/>
+    <n v="1657.7680499999999"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE3DB02C-6203-47E1-B75E-E7C71DA97B24}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="152">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="369">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="28"/>
+        <item sd="0" x="29"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="31"/>
+        <item sd="0" x="32"/>
+        <item sd="0" x="33"/>
+        <item sd="0" x="34"/>
+        <item sd="0" x="35"/>
+        <item sd="0" x="36"/>
+        <item sd="0" x="37"/>
+        <item sd="0" x="38"/>
+        <item sd="0" x="39"/>
+        <item sd="0" x="40"/>
+        <item sd="0" x="41"/>
+        <item sd="0" x="42"/>
+        <item sd="0" x="43"/>
+        <item sd="0" x="44"/>
+        <item sd="0" x="45"/>
+        <item sd="0" x="46"/>
+        <item sd="0" x="47"/>
+        <item sd="0" x="48"/>
+        <item sd="0" x="49"/>
+        <item sd="0" x="50"/>
+        <item sd="0" x="51"/>
+        <item sd="0" x="52"/>
+        <item sd="0" x="53"/>
+        <item sd="0" x="54"/>
+        <item sd="0" x="55"/>
+        <item sd="0" x="56"/>
+        <item sd="0" x="57"/>
+        <item sd="0" x="58"/>
+        <item sd="0" x="59"/>
+        <item sd="0" x="60"/>
+        <item sd="0" x="61"/>
+        <item sd="0" x="62"/>
+        <item sd="0" x="63"/>
+        <item sd="0" x="64"/>
+        <item sd="0" x="65"/>
+        <item sd="0" x="66"/>
+        <item sd="0" x="67"/>
+        <item sd="0" x="68"/>
+        <item sd="0" x="69"/>
+        <item sd="0" x="70"/>
+        <item sd="0" x="71"/>
+        <item sd="0" x="72"/>
+        <item sd="0" x="73"/>
+        <item sd="0" x="74"/>
+        <item sd="0" x="75"/>
+        <item sd="0" x="76"/>
+        <item sd="0" x="77"/>
+        <item sd="0" x="78"/>
+        <item sd="0" x="79"/>
+        <item sd="0" x="80"/>
+        <item sd="0" x="81"/>
+        <item sd="0" x="82"/>
+        <item sd="0" x="83"/>
+        <item sd="0" x="84"/>
+        <item sd="0" x="85"/>
+        <item sd="0" x="86"/>
+        <item sd="0" x="87"/>
+        <item sd="0" x="88"/>
+        <item sd="0" x="89"/>
+        <item sd="0" x="90"/>
+        <item sd="0" x="91"/>
+        <item sd="0" x="92"/>
+        <item sd="0" x="93"/>
+        <item sd="0" x="94"/>
+        <item sd="0" x="95"/>
+        <item sd="0" x="96"/>
+        <item sd="0" x="97"/>
+        <item sd="0" x="98"/>
+        <item sd="0" x="99"/>
+        <item sd="0" x="100"/>
+        <item sd="0" x="101"/>
+        <item sd="0" x="102"/>
+        <item sd="0" x="103"/>
+        <item sd="0" x="104"/>
+        <item sd="0" x="105"/>
+        <item sd="0" x="106"/>
+        <item sd="0" x="107"/>
+        <item sd="0" x="108"/>
+        <item sd="0" x="109"/>
+        <item sd="0" x="110"/>
+        <item sd="0" x="111"/>
+        <item sd="0" x="112"/>
+        <item sd="0" x="113"/>
+        <item sd="0" x="114"/>
+        <item sd="0" x="115"/>
+        <item sd="0" x="116"/>
+        <item sd="0" x="117"/>
+        <item sd="0" x="118"/>
+        <item sd="0" x="119"/>
+        <item sd="0" x="120"/>
+        <item sd="0" x="121"/>
+        <item sd="0" x="122"/>
+        <item sd="0" x="123"/>
+        <item sd="0" x="124"/>
+        <item sd="0" x="125"/>
+        <item sd="0" x="126"/>
+        <item sd="0" x="127"/>
+        <item sd="0" x="128"/>
+        <item sd="0" x="129"/>
+        <item sd="0" x="130"/>
+        <item sd="0" x="131"/>
+        <item sd="0" x="132"/>
+        <item sd="0" x="133"/>
+        <item sd="0" x="134"/>
+        <item sd="0" x="135"/>
+        <item sd="0" x="136"/>
+        <item sd="0" x="137"/>
+        <item sd="0" x="138"/>
+        <item sd="0" x="139"/>
+        <item sd="0" x="140"/>
+        <item sd="0" x="141"/>
+        <item sd="0" x="142"/>
+        <item sd="0" x="143"/>
+        <item sd="0" x="144"/>
+        <item sd="0" x="145"/>
+        <item sd="0" x="146"/>
+        <item sd="0" x="147"/>
+        <item sd="0" x="148"/>
+        <item sd="0" x="149"/>
+        <item sd="0" x="150"/>
+        <item sd="0" x="151"/>
+        <item sd="0" x="152"/>
+        <item sd="0" x="153"/>
+        <item sd="0" x="154"/>
+        <item sd="0" x="155"/>
+        <item sd="0" x="156"/>
+        <item sd="0" x="157"/>
+        <item sd="0" x="158"/>
+        <item sd="0" x="159"/>
+        <item sd="0" x="160"/>
+        <item sd="0" x="161"/>
+        <item sd="0" x="162"/>
+        <item sd="0" x="163"/>
+        <item sd="0" x="164"/>
+        <item sd="0" x="165"/>
+        <item sd="0" x="166"/>
+        <item sd="0" x="167"/>
+        <item sd="0" x="168"/>
+        <item sd="0" x="169"/>
+        <item sd="0" x="170"/>
+        <item sd="0" x="171"/>
+        <item sd="0" x="172"/>
+        <item sd="0" x="173"/>
+        <item sd="0" x="174"/>
+        <item sd="0" x="175"/>
+        <item sd="0" x="176"/>
+        <item sd="0" x="177"/>
+        <item sd="0" x="178"/>
+        <item sd="0" x="179"/>
+        <item sd="0" x="180"/>
+        <item sd="0" x="181"/>
+        <item sd="0" x="182"/>
+        <item sd="0" x="183"/>
+        <item sd="0" x="184"/>
+        <item sd="0" x="185"/>
+        <item sd="0" x="186"/>
+        <item sd="0" x="187"/>
+        <item sd="0" x="188"/>
+        <item sd="0" x="189"/>
+        <item sd="0" x="190"/>
+        <item sd="0" x="191"/>
+        <item sd="0" x="192"/>
+        <item sd="0" x="193"/>
+        <item sd="0" x="194"/>
+        <item sd="0" x="195"/>
+        <item sd="0" x="196"/>
+        <item sd="0" x="197"/>
+        <item sd="0" x="198"/>
+        <item sd="0" x="199"/>
+        <item sd="0" x="200"/>
+        <item sd="0" x="201"/>
+        <item sd="0" x="202"/>
+        <item sd="0" x="203"/>
+        <item sd="0" x="204"/>
+        <item sd="0" x="205"/>
+        <item sd="0" x="206"/>
+        <item sd="0" x="207"/>
+        <item sd="0" x="208"/>
+        <item sd="0" x="209"/>
+        <item sd="0" x="210"/>
+        <item sd="0" x="211"/>
+        <item sd="0" x="212"/>
+        <item sd="0" x="213"/>
+        <item sd="0" x="214"/>
+        <item sd="0" x="215"/>
+        <item sd="0" x="216"/>
+        <item sd="0" x="217"/>
+        <item sd="0" x="218"/>
+        <item sd="0" x="219"/>
+        <item sd="0" x="220"/>
+        <item sd="0" x="221"/>
+        <item sd="0" x="222"/>
+        <item sd="0" x="223"/>
+        <item sd="0" x="224"/>
+        <item sd="0" x="225"/>
+        <item sd="0" x="226"/>
+        <item sd="0" x="227"/>
+        <item sd="0" x="228"/>
+        <item sd="0" x="229"/>
+        <item sd="0" x="230"/>
+        <item sd="0" x="231"/>
+        <item sd="0" x="232"/>
+        <item sd="0" x="233"/>
+        <item sd="0" x="234"/>
+        <item sd="0" x="235"/>
+        <item sd="0" x="236"/>
+        <item sd="0" x="237"/>
+        <item sd="0" x="238"/>
+        <item sd="0" x="239"/>
+        <item sd="0" x="240"/>
+        <item sd="0" x="241"/>
+        <item sd="0" x="242"/>
+        <item sd="0" x="243"/>
+        <item sd="0" x="244"/>
+        <item sd="0" x="245"/>
+        <item sd="0" x="246"/>
+        <item sd="0" x="247"/>
+        <item sd="0" x="248"/>
+        <item sd="0" x="249"/>
+        <item sd="0" x="250"/>
+        <item sd="0" x="251"/>
+        <item sd="0" x="252"/>
+        <item sd="0" x="253"/>
+        <item sd="0" x="254"/>
+        <item sd="0" x="255"/>
+        <item sd="0" x="256"/>
+        <item sd="0" x="257"/>
+        <item sd="0" x="258"/>
+        <item sd="0" x="259"/>
+        <item sd="0" x="260"/>
+        <item sd="0" x="261"/>
+        <item sd="0" x="262"/>
+        <item sd="0" x="263"/>
+        <item sd="0" x="264"/>
+        <item sd="0" x="265"/>
+        <item sd="0" x="266"/>
+        <item sd="0" x="267"/>
+        <item sd="0" x="268"/>
+        <item sd="0" x="269"/>
+        <item sd="0" x="270"/>
+        <item sd="0" x="271"/>
+        <item sd="0" x="272"/>
+        <item sd="0" x="273"/>
+        <item sd="0" x="274"/>
+        <item sd="0" x="275"/>
+        <item sd="0" x="276"/>
+        <item sd="0" x="277"/>
+        <item sd="0" x="278"/>
+        <item sd="0" x="279"/>
+        <item sd="0" x="280"/>
+        <item sd="0" x="281"/>
+        <item sd="0" x="282"/>
+        <item sd="0" x="283"/>
+        <item sd="0" x="284"/>
+        <item sd="0" x="285"/>
+        <item sd="0" x="286"/>
+        <item sd="0" x="287"/>
+        <item sd="0" x="288"/>
+        <item sd="0" x="289"/>
+        <item sd="0" x="290"/>
+        <item sd="0" x="291"/>
+        <item sd="0" x="292"/>
+        <item sd="0" x="293"/>
+        <item sd="0" x="294"/>
+        <item sd="0" x="295"/>
+        <item sd="0" x="296"/>
+        <item sd="0" x="297"/>
+        <item sd="0" x="298"/>
+        <item sd="0" x="299"/>
+        <item sd="0" x="300"/>
+        <item sd="0" x="301"/>
+        <item sd="0" x="302"/>
+        <item sd="0" x="303"/>
+        <item sd="0" x="304"/>
+        <item sd="0" x="305"/>
+        <item sd="0" x="306"/>
+        <item sd="0" x="307"/>
+        <item sd="0" x="308"/>
+        <item sd="0" x="309"/>
+        <item sd="0" x="310"/>
+        <item sd="0" x="311"/>
+        <item sd="0" x="312"/>
+        <item sd="0" x="313"/>
+        <item sd="0" x="314"/>
+        <item sd="0" x="315"/>
+        <item sd="0" x="316"/>
+        <item sd="0" x="317"/>
+        <item sd="0" x="318"/>
+        <item sd="0" x="319"/>
+        <item sd="0" x="320"/>
+        <item sd="0" x="321"/>
+        <item sd="0" x="322"/>
+        <item sd="0" x="323"/>
+        <item sd="0" x="324"/>
+        <item sd="0" x="325"/>
+        <item sd="0" x="326"/>
+        <item sd="0" x="327"/>
+        <item sd="0" x="328"/>
+        <item sd="0" x="329"/>
+        <item sd="0" x="330"/>
+        <item sd="0" x="331"/>
+        <item sd="0" x="332"/>
+        <item sd="0" x="333"/>
+        <item sd="0" x="334"/>
+        <item sd="0" x="335"/>
+        <item sd="0" x="336"/>
+        <item sd="0" x="337"/>
+        <item sd="0" x="338"/>
+        <item sd="0" x="339"/>
+        <item sd="0" x="340"/>
+        <item sd="0" x="341"/>
+        <item sd="0" x="342"/>
+        <item sd="0" x="343"/>
+        <item sd="0" x="344"/>
+        <item sd="0" x="345"/>
+        <item sd="0" x="346"/>
+        <item sd="0" x="347"/>
+        <item sd="0" x="348"/>
+        <item sd="0" x="349"/>
+        <item sd="0" x="350"/>
+        <item sd="0" x="351"/>
+        <item sd="0" x="352"/>
+        <item sd="0" x="353"/>
+        <item sd="0" x="354"/>
+        <item sd="0" x="355"/>
+        <item sd="0" x="356"/>
+        <item sd="0" x="357"/>
+        <item sd="0" x="358"/>
+        <item sd="0" x="359"/>
+        <item sd="0" x="360"/>
+        <item sd="0" x="361"/>
+        <item sd="0" x="362"/>
+        <item sd="0" x="363"/>
+        <item sd="0" x="364"/>
+        <item sd="0" x="365"/>
+        <item sd="0" x="366"/>
+        <item sd="0" x="367"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="8"/>
+    <field x="7"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Suma de Ventas totales" fld="1" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="% ventas" fld="1" showDataAs="percentOfCol" baseField="8" baseItem="1" numFmtId="10"/>
+    <dataField name="Promedio de Tickets" fld="6" subtotal="average" baseField="8" baseItem="1" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,11 +3328,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0A6887-8475-424B-9734-280674815BD8}">
+  <dimension ref="A3:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11">
+        <v>123191.02</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.20292728127563853</v>
+      </c>
+      <c r="D4" s="13">
+        <v>39.225806451612904</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="11">
+        <v>110688.44</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.18233231771148284</v>
+      </c>
+      <c r="D5" s="13">
+        <v>36.607142857142854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11">
+        <v>121427.19</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.20002179980034585</v>
+      </c>
+      <c r="D6" s="13">
+        <v>36.258064516129032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="11">
+        <v>118557.21</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.19529420489354618</v>
+      </c>
+      <c r="D7" s="13">
+        <v>36.666666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="11">
+        <v>133205.91999999998</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.21942439631898655</v>
+      </c>
+      <c r="D8" s="13">
+        <v>36.516129032258064</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11">
+        <v>607069.78</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>37.066225165562912</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C0ADA3-4C22-4CF9-8AD3-3A127D5F6CB1}">
   <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4278,11 +7059,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A23CDF-F090-4714-AB49-78B50071C889}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -4482,7 +7263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B68A6B-4F66-49B3-AEDB-48F8AD760459}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -4623,7 +7404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A9D3D7-F34D-4A34-8B58-0EC02683C78D}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -4842,7 +7623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF169ED-0A5B-4E85-A1DC-CF4116D4BB32}">
   <dimension ref="B2:H3"/>
   <sheetViews>

</xml_diff>